<commit_message>
changes to how vertex settings computed.
</commit_message>
<xml_diff>
--- a/test_graph_analysis/data_test/Sample Equations.xlsx
+++ b/test_graph_analysis/data_test/Sample Equations.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bc151\Documents\Toolsmithing\ricks-cafe-american\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconnelly7-gtri\Documents\Ingrid_Nerdman\test_graph_analysis\data_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Parametric" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -486,21 +486,21 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.59765625" customWidth="1"/>
-    <col min="2" max="2" width="21.86328125" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="3" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="36.73046875" customWidth="1"/>
-    <col min="6" max="8" width="21.86328125" customWidth="1"/>
-    <col min="9" max="9" width="42.59765625" customWidth="1"/>
-    <col min="10" max="13" width="13.86328125" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" customWidth="1"/>
+    <col min="6" max="8" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="42.5703125" customWidth="1"/>
+    <col min="10" max="13" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,7 +529,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -558,7 +558,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -587,7 +587,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -616,7 +616,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -645,7 +645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -674,7 +674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -703,7 +703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -732,7 +732,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -761,7 +761,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>

</xml_diff>